<commit_message>
Add test cases for Registration Scenario
</commit_message>
<xml_diff>
--- a/Test cases/Test cases for E-commerce .xlsx
+++ b/Test cases/Test cases for E-commerce .xlsx
@@ -1,23 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{77D57CCF-2FF3-4433-A664-38A68F688560}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\QA\Git\Projects\Test-documentation\Test cases\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3463A2E-A8A3-4393-B405-FC31CFCA2A8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Test cases" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
@@ -27,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="52">
   <si>
     <t>ID</t>
   </si>
@@ -111,13 +114,105 @@
   </si>
   <si>
     <t>TC16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Registration with valid data </t>
+  </si>
+  <si>
+    <t>n/a</t>
+  </si>
+  <si>
+    <t>E-mail:Inat1952@gustr.com
+Password:1234567890</t>
+  </si>
+  <si>
+    <t>1.Go to https://dominos.ua/uk/kyiv/
+2.Click on "Увійти" button
+3.Click on "Registration" button
+4.Click on "Зареєструватися" button(without filling any fields)</t>
+  </si>
+  <si>
+    <t>Registration without any data provided</t>
+  </si>
+  <si>
+    <t>Registration with invalid email provided</t>
+  </si>
+  <si>
+    <t>E-mail:Inat1952gustr.com
+Password:1234567890</t>
+  </si>
+  <si>
+    <t>User is not logged in</t>
+  </si>
+  <si>
+    <t>Registration with invalid password provided</t>
+  </si>
+  <si>
+    <t>E-mail:Inat1952@gustr.com
+Password:1234</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Registration with invalid password confirmation data provided </t>
+  </si>
+  <si>
+    <t>E-mail:Inat1952@gustr.com
+Password:1234567890
+Confirmation password:qwertyui</t>
+  </si>
+  <si>
+    <t>1.User have account 
+2.User is not logged in</t>
+  </si>
+  <si>
+    <t>TC17</t>
+  </si>
+  <si>
+    <t>1.Go to https://dominos.ua/uk/kyiv/
+2.Click on "Увійти" button
+3.Click on "Registration" button
+4.Fill out "Ваш email", "Пароль" and "Повторіть ваш пароль"  fields
+5.Click on "Зареєструватися"</t>
+  </si>
+  <si>
+    <t>1.Create an email(e.g. here www.fakemailgenerator.com)
+2.User is not logged in</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.Go to https://dominos.ua/uk/kyiv/
+2.Click on "Увійти" button
+3.Click on "Registration" button
+4.Fill out "Ваш email", "Пароль" and "Повторіть ваш пароль"  fields
+5.Click on "Зареєструватися" button
+6. Go to mailbox used during registration and find a welcome letter
+7.Click on "Підтвердити" link </t>
+  </si>
+  <si>
+    <t>User will not be registered and all fields will be marked in red and message "Це поле є обов'язковим." near each field will be displayed</t>
+  </si>
+  <si>
+    <t>User will not be registered, "Ваш email" field will be marked in red and message "Введіть коректну адресу електронної пошти." will be displayed</t>
+  </si>
+  <si>
+    <t>User will not be registered, "Пароль" and "Повторіть пароль" fields will be marked in red and message "Переконайтесь, що в цьому полі мінімум 8 символів." will be displayed</t>
+  </si>
+  <si>
+    <t>User will not be registered, "Повторіть пароль" field will be marked in red and message "Паролі не співпадають" will be displayed</t>
+  </si>
+  <si>
+    <t>Registration with registered email</t>
+  </si>
+  <si>
+    <t>User will not be registered, "Ваш email" field will be marked in red and message "Аккаунт с таким email вже існує" will be displayed</t>
+  </si>
+  <si>
+    <t>User will be redirected to the site to profile page, tab "Реєстрація в програмі лояльності"  will be displayed</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -142,6 +237,18 @@
       <color theme="1"/>
       <name val="Times New Roman"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -164,13 +271,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFF2CC"/>
+        <fgColor theme="7" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC9DAF8"/>
+        <fgColor theme="4" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -215,7 +322,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" readingOrder="1"/>
@@ -227,12 +334,6 @@
       <alignment horizontal="center" vertical="center" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -240,9 +341,42 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Звичайний" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -554,26 +688,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I17"/>
+  <dimension ref="A1:I18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.7109375" style="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.7109375" style="7" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5" style="7" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.7109375" style="7" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.28515625" style="7" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.140625" style="7" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.42578125" style="7" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.42578125" style="7" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="7"/>
+    <col min="1" max="1" width="5.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="54.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.42578125" style="5" customWidth="1"/>
+    <col min="5" max="5" width="27.5703125" style="5" customWidth="1"/>
+    <col min="6" max="6" width="64.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="32.7109375" style="5" customWidth="1"/>
+    <col min="8" max="8" width="25" style="5" customWidth="1"/>
+    <col min="9" max="9" width="36" style="5" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15.75">
+    <row r="1" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -602,98 +737,158 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" ht="105" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>9</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="9"/>
-      <c r="H2" s="9"/>
-      <c r="I2" s="8"/>
-    </row>
-    <row r="3" spans="1:9">
+      <c r="C2" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D2" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="F2" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="G2" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="H2" s="7"/>
+      <c r="I2" s="6"/>
+    </row>
+    <row r="3" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>11</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="9"/>
-      <c r="H3" s="9"/>
-      <c r="I3" s="8"/>
-    </row>
-    <row r="4" spans="1:9">
+      <c r="C3" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F3" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="G3" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="H3" s="7"/>
+      <c r="I3" s="6"/>
+    </row>
+    <row r="4" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="9"/>
-      <c r="H4" s="9"/>
-      <c r="I4" s="8"/>
-    </row>
-    <row r="5" spans="1:9">
+      <c r="C4" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="F4" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="G4" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="H4" s="7"/>
+      <c r="I4" s="6"/>
+    </row>
+    <row r="5" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>13</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="9"/>
-      <c r="H5" s="9"/>
-      <c r="I5" s="8"/>
-    </row>
-    <row r="6" spans="1:9">
+      <c r="C5" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="F5" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="G5" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="H5" s="7"/>
+      <c r="I5" s="6"/>
+    </row>
+    <row r="6" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>14</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="9"/>
-      <c r="H6" s="9"/>
-      <c r="I6" s="8"/>
-    </row>
-    <row r="7" spans="1:9">
-      <c r="A7" s="5" t="s">
+      <c r="C6" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D6" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="E6" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="F6" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="G6" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="H6" s="7"/>
+      <c r="I6" s="6"/>
+    </row>
+    <row r="7" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="9"/>
-      <c r="H7" s="9"/>
-      <c r="I7" s="8"/>
-    </row>
-    <row r="8" spans="1:9">
-      <c r="A8" s="5" t="s">
+      <c r="B7" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="D7" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="E7" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="F7" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="G7" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="H7" s="7"/>
+      <c r="I7" s="6"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="17" t="s">
         <v>17</v>
       </c>
       <c r="B8" s="4" t="s">
@@ -702,13 +897,13 @@
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="9"/>
-      <c r="H8" s="9"/>
-      <c r="I8" s="8"/>
-    </row>
-    <row r="9" spans="1:9">
-      <c r="A9" s="5" t="s">
+      <c r="F8" s="11"/>
+      <c r="G8" s="10"/>
+      <c r="H8" s="7"/>
+      <c r="I8" s="6"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="17" t="s">
         <v>18</v>
       </c>
       <c r="B9" s="4" t="s">
@@ -717,13 +912,13 @@
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="9"/>
-      <c r="H9" s="9"/>
-      <c r="I9" s="8"/>
-    </row>
-    <row r="10" spans="1:9">
-      <c r="A10" s="5" t="s">
+      <c r="F9" s="11"/>
+      <c r="G9" s="10"/>
+      <c r="H9" s="7"/>
+      <c r="I9" s="6"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="17" t="s">
         <v>19</v>
       </c>
       <c r="B10" s="4" t="s">
@@ -732,13 +927,13 @@
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="9"/>
-      <c r="H10" s="9"/>
-      <c r="I10" s="8"/>
-    </row>
-    <row r="11" spans="1:9">
-      <c r="A11" s="5" t="s">
+      <c r="F10" s="11"/>
+      <c r="G10" s="10"/>
+      <c r="H10" s="7"/>
+      <c r="I10" s="6"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="17" t="s">
         <v>20</v>
       </c>
       <c r="B11" s="4" t="s">
@@ -747,13 +942,13 @@
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="9"/>
-      <c r="H11" s="9"/>
-      <c r="I11" s="8"/>
-    </row>
-    <row r="12" spans="1:9">
-      <c r="A12" s="5" t="s">
+      <c r="F11" s="11"/>
+      <c r="G11" s="10"/>
+      <c r="H11" s="7"/>
+      <c r="I11" s="6"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="17" t="s">
         <v>21</v>
       </c>
       <c r="B12" s="4" t="s">
@@ -762,28 +957,28 @@
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-      <c r="G12" s="9"/>
-      <c r="H12" s="9"/>
-      <c r="I12" s="8"/>
-    </row>
-    <row r="13" spans="1:9">
-      <c r="A13" s="6" t="s">
+      <c r="F12" s="11"/>
+      <c r="G12" s="10"/>
+      <c r="H12" s="7"/>
+      <c r="I12" s="6"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="17" t="s">
         <v>22</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
-      <c r="G13" s="9"/>
-      <c r="H13" s="9"/>
-      <c r="I13" s="8"/>
-    </row>
-    <row r="14" spans="1:9">
-      <c r="A14" s="6" t="s">
+      <c r="F13" s="11"/>
+      <c r="G13" s="10"/>
+      <c r="H13" s="7"/>
+      <c r="I13" s="6"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="18" t="s">
         <v>24</v>
       </c>
       <c r="B14" s="4" t="s">
@@ -792,13 +987,13 @@
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
-      <c r="G14" s="9"/>
-      <c r="H14" s="9"/>
-      <c r="I14" s="8"/>
-    </row>
-    <row r="15" spans="1:9">
-      <c r="A15" s="6" t="s">
+      <c r="F14" s="11"/>
+      <c r="G14" s="10"/>
+      <c r="H14" s="7"/>
+      <c r="I14" s="6"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="18" t="s">
         <v>25</v>
       </c>
       <c r="B15" s="4" t="s">
@@ -807,13 +1002,13 @@
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
-      <c r="G15" s="9"/>
-      <c r="H15" s="9"/>
-      <c r="I15" s="8"/>
-    </row>
-    <row r="16" spans="1:9">
-      <c r="A16" s="6" t="s">
+      <c r="F15" s="11"/>
+      <c r="G15" s="10"/>
+      <c r="H15" s="7"/>
+      <c r="I15" s="6"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="18" t="s">
         <v>26</v>
       </c>
       <c r="B16" s="4" t="s">
@@ -822,13 +1017,13 @@
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
-      <c r="G16" s="9"/>
-      <c r="H16" s="9"/>
-      <c r="I16" s="8"/>
-    </row>
-    <row r="17" spans="1:9">
-      <c r="A17" s="6" t="s">
+      <c r="F16" s="11"/>
+      <c r="G16" s="10"/>
+      <c r="H16" s="7"/>
+      <c r="I16" s="6"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" s="18" t="s">
         <v>27</v>
       </c>
       <c r="B17" s="4" t="s">
@@ -837,12 +1032,29 @@
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
-      <c r="F17" s="2"/>
-      <c r="G17" s="9"/>
-      <c r="H17" s="9"/>
-      <c r="I17" s="8"/>
+      <c r="F17" s="11"/>
+      <c r="G17" s="10"/>
+      <c r="H17" s="7"/>
+      <c r="I17" s="6"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="11"/>
+      <c r="G18" s="10"/>
+      <c r="H18" s="7"/>
+      <c r="I18" s="6"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add test cases for Logging in
</commit_message>
<xml_diff>
--- a/Test cases/Test cases for E-commerce .xlsx
+++ b/Test cases/Test cases for E-commerce .xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\QA\Git\Projects\Test-documentation\Test cases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3463A2E-A8A3-4393-B405-FC31CFCA2A8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73F836A5-6640-4AD4-B219-FAEB85858476}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="78">
   <si>
     <t>ID</t>
   </si>
@@ -99,9 +99,6 @@
   </si>
   <si>
     <t>TC12</t>
-  </si>
-  <si>
-    <t>Search Engine</t>
   </si>
   <si>
     <t>TC13</t>
@@ -126,16 +123,7 @@
 Password:1234567890</t>
   </si>
   <si>
-    <t>1.Go to https://dominos.ua/uk/kyiv/
-2.Click on "Увійти" button
-3.Click on "Registration" button
-4.Click on "Зареєструватися" button(without filling any fields)</t>
-  </si>
-  <si>
     <t>Registration without any data provided</t>
-  </si>
-  <si>
-    <t>Registration with invalid email provided</t>
   </si>
   <si>
     <t>E-mail:Inat1952gustr.com
@@ -160,22 +148,7 @@
 Confirmation password:qwertyui</t>
   </si>
   <si>
-    <t>1.User have account 
-2.User is not logged in</t>
-  </si>
-  <si>
     <t>TC17</t>
-  </si>
-  <si>
-    <t>1.Go to https://dominos.ua/uk/kyiv/
-2.Click on "Увійти" button
-3.Click on "Registration" button
-4.Fill out "Ваш email", "Пароль" and "Повторіть ваш пароль"  fields
-5.Click on "Зареєструватися"</t>
-  </si>
-  <si>
-    <t>1.Create an email(e.g. here www.fakemailgenerator.com)
-2.User is not logged in</t>
   </si>
   <si>
     <t xml:space="preserve">1.Go to https://dominos.ua/uk/kyiv/
@@ -187,25 +160,147 @@
 7.Click on "Підтвердити" link </t>
   </si>
   <si>
-    <t>User will not be registered and all fields will be marked in red and message "Це поле є обов'язковим." near each field will be displayed</t>
-  </si>
-  <si>
-    <t>User will not be registered, "Ваш email" field will be marked in red and message "Введіть коректну адресу електронної пошти." will be displayed</t>
-  </si>
-  <si>
-    <t>User will not be registered, "Пароль" and "Повторіть пароль" fields will be marked in red and message "Переконайтесь, що в цьому полі мінімум 8 символів." will be displayed</t>
-  </si>
-  <si>
-    <t>User will not be registered, "Повторіть пароль" field will be marked in red and message "Паролі не співпадають" will be displayed</t>
-  </si>
-  <si>
-    <t>Registration with registered email</t>
-  </si>
-  <si>
-    <t>User will not be registered, "Ваш email" field will be marked in red and message "Аккаунт с таким email вже існує" will be displayed</t>
-  </si>
-  <si>
-    <t>User will be redirected to the site to profile page, tab "Реєстрація в програмі лояльності"  will be displayed</t>
+    <t>Logging in with valid data</t>
+  </si>
+  <si>
+    <t>1.User have account on https://dominos.ua/uk/kyiv/
+2.User is not logged in</t>
+  </si>
+  <si>
+    <t>User have account on https://dominos.ua/uk/kyiv/</t>
+  </si>
+  <si>
+    <t>1.Go to https://dominos.ua/uk/kyiv/
+2.Click on "Увійти" button
+3.Click on "Registration" button
+4.Fill out "Ваш email", "Пароль" and "Повторіть ваш пароль"  fields
+5.Click on "Зареєструватися" button</t>
+  </si>
+  <si>
+    <t>User is redirected to the site to profile page, tab "Реєстрація в програмі лояльності" is displayed</t>
+  </si>
+  <si>
+    <t>User is not registered and all fields are marked in red and message "Це поле є обов'язковим." near each field is displayed</t>
+  </si>
+  <si>
+    <t>User is not registered, "Ваш email" field is marked in red and message "Введіть коректну адресу електронної пошти." is displayed</t>
+  </si>
+  <si>
+    <t>User will is not registered, "Пароль" and "Повторіть пароль" fields are marked in red and message "Переконайтесь, що в цьому полі мінімум 8 символів." is displayed</t>
+  </si>
+  <si>
+    <t>User is not be registered, "Повторіть пароль" field is marked in red and message "Паролі не співпадають" is displayed</t>
+  </si>
+  <si>
+    <t>User is logged in and redirected to the main page</t>
+  </si>
+  <si>
+    <t>Logging in without any data provided</t>
+  </si>
+  <si>
+    <t>1.Go to https://dominos.ua/uk/kyiv/
+2.Click on "Увійти" button
+3.Click on "Увійти" button(without filling any field)</t>
+  </si>
+  <si>
+    <t>1.Go to https://dominos.ua/uk/kyiv/
+2.Click on "Увійти" button
+3.Click on "Registration" button
+4.Click on "Зареєструватися" button(without filling any field)</t>
+  </si>
+  <si>
+    <t>User is not logged in, each field is marked in red and message "Це поле є обов'язковим." is displayed near each field</t>
+  </si>
+  <si>
+    <t>User do not have account on https://dominos.ua/uk/kyiv/</t>
+  </si>
+  <si>
+    <t>User is not logged in, "Логін" field is marked in red and message "Користувача з таким email не знайдено" is displayed</t>
+  </si>
+  <si>
+    <t>E-mail:Inat1952@gustr.com</t>
+  </si>
+  <si>
+    <t>E-mail:testemail@gustr.com
+Password:test1234</t>
+  </si>
+  <si>
+    <t>E-mail:Inat1952@gustr.com
+Password:test1234</t>
+  </si>
+  <si>
+    <t>User is not logged in, "Пароль" field is marked in red and message "Невірний пароль" is displayed</t>
+  </si>
+  <si>
+    <t>1.Create an E-mail(e.g. here www.fakemailgenerator.com)
+2.User is not logged in</t>
+  </si>
+  <si>
+    <t>Registration with invalid E-mail provided</t>
+  </si>
+  <si>
+    <t>Registration with registered E-mail</t>
+  </si>
+  <si>
+    <t>1.Go to https://dominos.ua/uk/kyiv/
+2.Click on "Увійти" button
+3.Fill out "Логін"(E-mail) and" Пароль" fields 
+4.Click on "Увійти" button</t>
+  </si>
+  <si>
+    <t>Restoring password with E-mail that exist in the system</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.Go to https://dominos.ua/uk/kyiv/
+2.Click on "Увійти" button
+3.Click on "Забули пароль?" button
+4.Filling out "E-mail" field  in popped up window 
+5.Click on "Підтвердити" button
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">User receive following message "Посилання на вхід було відправлено на вашу email адресу" and letter with "Логін" link to enter the profile on site
+</t>
+  </si>
+  <si>
+    <t>Restoring password with E-mail that does not exist in the system</t>
+  </si>
+  <si>
+    <t>E-mail:testemail@gustr.com</t>
+  </si>
+  <si>
+    <t>1.Go to https://dominos.ua/uk/kyiv/
+2.Click on "Увійти" button
+3.Click on "Забули пароль?" button
+4.Filling out "E-mail" field  in popped up window 
+5.Click on "Підтвердити" button</t>
+  </si>
+  <si>
+    <t>User is not be registered, "Ваш email" field is marked in red and message "Аккаунт з таким email вже існує" is displayed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"Email" field is marked in red and message "Email не знайдено" is displayed </t>
+  </si>
+  <si>
+    <t>Shopping cart</t>
+  </si>
+  <si>
+    <t>Adding product to the cart</t>
+  </si>
+  <si>
+    <t>Removing product from the cart</t>
+  </si>
+  <si>
+    <t>Changing quantity of the items in the cart</t>
+  </si>
+  <si>
+    <t>Removing product from the cart through changing quantity by clicking increase/decrease button</t>
+  </si>
+  <si>
+    <t>Logging in with data that does not exist in the system</t>
+  </si>
+  <si>
+    <t>Logging in with existing E-mail, but invalid password</t>
   </si>
 </sst>
 </file>
@@ -322,7 +417,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" readingOrder="1"/>
@@ -373,6 +468,12 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -690,16 +791,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5.7109375" style="5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="54.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.42578125" style="5" customWidth="1"/>
+    <col min="3" max="3" width="56.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.42578125" style="20" customWidth="1"/>
     <col min="5" max="5" width="27.5703125" style="5" customWidth="1"/>
     <col min="6" max="6" width="64.85546875" style="5" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="32.7109375" style="5" customWidth="1"/>
@@ -718,7 +820,7 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="19" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
@@ -745,19 +847,19 @@
         <v>10</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D2" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="F2" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="G2" s="12" t="s">
         <v>43</v>
-      </c>
-      <c r="E2" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="F2" s="14" t="s">
-        <v>44</v>
-      </c>
-      <c r="G2" s="12" t="s">
-        <v>51</v>
       </c>
       <c r="H2" s="7"/>
       <c r="I2" s="6"/>
@@ -770,19 +872,19 @@
         <v>10</v>
       </c>
       <c r="C3" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D3" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>35</v>
-      </c>
       <c r="E3" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F3" s="9" t="s">
-        <v>31</v>
+        <v>51</v>
       </c>
       <c r="G3" s="12" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H3" s="7"/>
       <c r="I3" s="6"/>
@@ -795,24 +897,24 @@
         <v>10</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>35</v>
+        <v>60</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>32</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="F4" s="14" t="s">
         <v>42</v>
       </c>
       <c r="G4" s="12" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H4" s="7"/>
       <c r="I4" s="6"/>
     </row>
-    <row r="5" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>13</v>
       </c>
@@ -820,19 +922,19 @@
         <v>10</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>32</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="F5" s="14" t="s">
         <v>42</v>
       </c>
       <c r="G5" s="12" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H5" s="7"/>
       <c r="I5" s="6"/>
@@ -845,19 +947,19 @@
         <v>10</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="D6" s="16" t="s">
         <v>35</v>
       </c>
+      <c r="D6" s="13" t="s">
+        <v>32</v>
+      </c>
       <c r="E6" s="13" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="F6" s="14" t="s">
         <v>42</v>
       </c>
       <c r="G6" s="12" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H6" s="7"/>
       <c r="I6" s="6"/>
@@ -870,122 +972,184 @@
         <v>10</v>
       </c>
       <c r="C7" s="16" t="s">
-        <v>49</v>
+        <v>61</v>
       </c>
       <c r="D7" s="13" t="s">
         <v>40</v>
       </c>
       <c r="E7" s="13" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F7" s="14" t="s">
         <v>42</v>
       </c>
       <c r="G7" s="12" t="s">
-        <v>50</v>
+        <v>69</v>
       </c>
       <c r="H7" s="7"/>
       <c r="I7" s="6"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A8" s="17" t="s">
         <v>17</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="11"/>
-      <c r="G8" s="10"/>
+      <c r="C8" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="E8" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="F8" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="G8" s="10" t="s">
+        <v>48</v>
+      </c>
       <c r="H8" s="7"/>
       <c r="I8" s="6"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A9" s="17" t="s">
         <v>18</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="11"/>
-      <c r="G9" s="10"/>
+      <c r="C9" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F9" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="G9" s="10" t="s">
+        <v>52</v>
+      </c>
       <c r="H9" s="7"/>
       <c r="I9" s="6"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A10" s="17" t="s">
         <v>19</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="11"/>
-      <c r="G10" s="10"/>
+      <c r="C10" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="F10" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="G10" s="10" t="s">
+        <v>54</v>
+      </c>
       <c r="H10" s="7"/>
       <c r="I10" s="6"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A11" s="17" t="s">
         <v>20</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="11"/>
-      <c r="G11" s="10"/>
+      <c r="C11" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="E11" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="F11" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="G11" s="10" t="s">
+        <v>58</v>
+      </c>
       <c r="H11" s="7"/>
       <c r="I11" s="6"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A12" s="17" t="s">
         <v>21</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="11"/>
-      <c r="G12" s="10"/>
+      <c r="C12" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="F12" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="G12" s="10" t="s">
+        <v>65</v>
+      </c>
       <c r="H12" s="7"/>
       <c r="I12" s="6"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A13" s="17" t="s">
         <v>22</v>
       </c>
       <c r="B13" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="11"/>
-      <c r="G13" s="10"/>
+      <c r="C13" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="F13" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="G13" s="10" t="s">
+        <v>70</v>
+      </c>
       <c r="H13" s="7"/>
       <c r="I13" s="6"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="18" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
+        <v>71</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="D14" s="8"/>
       <c r="E14" s="2"/>
       <c r="F14" s="11"/>
       <c r="G14" s="10"/>
@@ -994,13 +1158,15 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="18" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
+        <v>71</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="D15" s="8"/>
       <c r="E15" s="2"/>
       <c r="F15" s="11"/>
       <c r="G15" s="10"/>
@@ -1009,28 +1175,32 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="18" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
+        <v>71</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="D16" s="8"/>
       <c r="E16" s="2"/>
       <c r="F16" s="11"/>
       <c r="G16" s="10"/>
       <c r="H16" s="7"/>
       <c r="I16" s="6"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="18" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
+        <v>71</v>
+      </c>
+      <c r="C17" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="D17" s="8"/>
       <c r="E17" s="2"/>
       <c r="F17" s="11"/>
       <c r="G17" s="10"/>
@@ -1039,13 +1209,13 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="18" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>23</v>
+        <v>71</v>
       </c>
       <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
+      <c r="D18" s="8"/>
       <c r="E18" s="2"/>
       <c r="F18" s="11"/>
       <c r="G18" s="10"/>

</xml_diff>

<commit_message>
Add test cases for Logging in scenario
</commit_message>
<xml_diff>
--- a/Test cases/Test cases for E-commerce .xlsx
+++ b/Test cases/Test cases for E-commerce .xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\QA\Git\Projects\Test-documentation\Test cases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73F836A5-6640-4AD4-B219-FAEB85858476}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A032B930-C216-4B0F-AF7B-44E35A9B7328}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -792,8 +792,8 @@
   <dimension ref="A1:I18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D17" sqref="D17"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>